<commit_message>
update to version 1.0.2
</commit_message>
<xml_diff>
--- a/column_definitions.xlsx
+++ b/column_definitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateoforegon-my.sharepoint.com/personal/ryan_michie_deq_oregon_gov/Documents/GitHub/odeqtmdlquery/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{8E9C8C05-3E5D-4B4A-BA53-7C7E16A664B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14489FEA-95DC-402E-9BC9-3C0A023C959B}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{8E9C8C05-3E5D-4B4A-BA53-7C7E16A664B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C175781-088F-42F7-B452-3CF3A31DB915}"/>
   <bookViews>
-    <workbookView xWindow="708" yWindow="0" windowWidth="22332" windowHeight="12504" xr2:uid="{1BB4F8A1-4779-4200-A825-E2E2DE8ECC5A}"/>
+    <workbookView xWindow="5850" yWindow="1410" windowWidth="39315" windowHeight="17475" xr2:uid="{1BB4F8A1-4779-4200-A825-E2E2DE8ECC5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Column_Descriptions" sheetId="1" r:id="rId1"/>
@@ -474,9 +474,6 @@
     <t>Name of TMDL document (agency, year TMDL was issued)</t>
   </si>
   <si>
-    <t>Note summarizing high level information about the TMDL overall. Comments about TMDL parameter status go in the TMDL_status_comment.</t>
-  </si>
-  <si>
     <t>The total count of TMDL assessment units matching the query. One TMDL is equal to one assessment unit for one 303(d) water quality parameter. If two different 303(d) water quality parameters are applicable to the same assessment unit, they are counted as two TMDLs. The TMDL count includes any assessment units addressed by the TMDL action, regardless of that assessment unit's status on the Integrated Report.</t>
   </si>
   <si>
@@ -486,9 +483,6 @@
     <t>R pacakge version</t>
   </si>
   <si>
-    <t>0.9.10</t>
-  </si>
-  <si>
     <t>Provides information about how the TMDL applies</t>
   </si>
   <si>
@@ -505,6 +499,12 @@
   </si>
   <si>
     <t>Point Source WLAs</t>
+  </si>
+  <si>
+    <t>Note summarizing general information about the TMDL overall.</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
   </si>
 </sst>
 </file>
@@ -927,19 +927,19 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -953,9 +953,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>1</v>
@@ -964,9 +964,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>2</v>
@@ -975,9 +975,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>3</v>
@@ -986,9 +986,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>4</v>
@@ -997,9 +997,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>5</v>
@@ -1011,20 +1011,20 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>7</v>
@@ -1033,9 +1033,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>8</v>
@@ -1044,31 +1044,31 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>11</v>
@@ -1077,9 +1077,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>13</v>
@@ -1088,9 +1088,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>14</v>
@@ -1099,9 +1099,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>15</v>
@@ -1110,9 +1110,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>16</v>
@@ -1121,9 +1121,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>17</v>
@@ -1132,9 +1132,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>18</v>
@@ -1143,9 +1143,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>19</v>
@@ -1154,9 +1154,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>20</v>
@@ -1165,9 +1165,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>21</v>
@@ -1176,9 +1176,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>22</v>
@@ -1190,9 +1190,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>23</v>
@@ -1201,9 +1201,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>1</v>
@@ -1212,9 +1212,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>4</v>
@@ -1223,9 +1223,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>24</v>
@@ -1234,9 +1234,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>25</v>
@@ -1245,9 +1245,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>26</v>
@@ -1256,9 +1256,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>27</v>
@@ -1267,9 +1267,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>28</v>
@@ -1278,23 +1278,23 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="390" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>30</v>
@@ -1306,9 +1306,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>31</v>
@@ -1317,9 +1317,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>32</v>
@@ -1328,9 +1328,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>1</v>
@@ -1339,9 +1339,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>4</v>
@@ -1350,9 +1350,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>33</v>
@@ -1361,9 +1361,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>34</v>
@@ -1372,9 +1372,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>27</v>
@@ -1383,9 +1383,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>28</v>
@@ -1394,23 +1394,23 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="390" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>30</v>
@@ -1422,9 +1422,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>35</v>
@@ -1433,9 +1433,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>36</v>
@@ -1444,9 +1444,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>1</v>
@@ -1455,9 +1455,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>4</v>
@@ -1466,9 +1466,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>37</v>
@@ -1477,9 +1477,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>38</v>
@@ -1488,9 +1488,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>39</v>
@@ -1499,9 +1499,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>24</v>
@@ -1510,9 +1510,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>28</v>
@@ -1521,9 +1521,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>1</v>
@@ -1532,9 +1532,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>4</v>
@@ -1553,22 +1553,22 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>